<commit_message>
About page updated with general tests
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 AboutPage, Kevin O'Hare.xlsx
+++ b/Testing Spreadsheet v1.0 AboutPage, Kevin O'Hare.xlsx
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="236">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -434,15 +434,6 @@
     <t>4.1.21</t>
   </si>
   <si>
-    <t>To show that selecing the 2nd quick pizza link opens it in another tab/window</t>
-  </si>
-  <si>
-    <t>To show that selecing the 1st quick pizza link opens it in another tab/window</t>
-  </si>
-  <si>
-    <t>To show that selecing the 3rd quick pizza link opens it in another tab/window</t>
-  </si>
-  <si>
     <t>To show that when Order is selected as a non-logged in user on the About page, the user is prevented from accessing the Order page</t>
   </si>
   <si>
@@ -789,6 +780,165 @@
   </si>
   <si>
     <t>Log in using a valid username and password, direct to the About page and then direct to the Order page.</t>
+  </si>
+  <si>
+    <t>To show that selecting the 1st quick pizza link opens it in another tab/window</t>
+  </si>
+  <si>
+    <t>To show that selecting the 2nd quick pizza link opens it in another tab/window</t>
+  </si>
+  <si>
+    <t>To show that selecting the 3rd quick pizza link opens it in another tab/window</t>
+  </si>
+  <si>
+    <t>4.1.5</t>
+  </si>
+  <si>
+    <t>About_Tconn_14</t>
+  </si>
+  <si>
+    <t>To show that the About page exists as part of the website system</t>
+  </si>
+  <si>
+    <t>4.1.9</t>
+  </si>
+  <si>
+    <t>About_Tconn_15</t>
+  </si>
+  <si>
+    <t>4.1.10</t>
+  </si>
+  <si>
+    <t>4.1.11</t>
+  </si>
+  <si>
+    <t>About_Tconn_16</t>
+  </si>
+  <si>
+    <t>About_Tconn_17</t>
+  </si>
+  <si>
+    <t>About_Tconn_18</t>
+  </si>
+  <si>
+    <t>To show that a non-logged in user can directly navigate to the "Register" and "Log in" pages from the "About" page</t>
+  </si>
+  <si>
+    <t>To show that a logged in user can directly navigate to the "My Account - reset password" page from the "About" page</t>
+  </si>
+  <si>
+    <t>To show that a logged in user can log off from the "About" page</t>
+  </si>
+  <si>
+    <t>To show that the "Forgot password" page is not directly accessible from the "About" page</t>
+  </si>
+  <si>
+    <t>Check if the About page exists as part of the website</t>
+  </si>
+  <si>
+    <t>Nav_TCon_14</t>
+  </si>
+  <si>
+    <t>TCase_14</t>
+  </si>
+  <si>
+    <t>About_TProc_14</t>
+  </si>
+  <si>
+    <t>While on the website system, check if the About page exists</t>
+  </si>
+  <si>
+    <t>About page is accessible and displays when selected</t>
+  </si>
+  <si>
+    <t>About_TProc_15</t>
+  </si>
+  <si>
+    <t>TCase_15</t>
+  </si>
+  <si>
+    <t>About_TProc_16</t>
+  </si>
+  <si>
+    <t>TCase_16</t>
+  </si>
+  <si>
+    <t>TCase_17</t>
+  </si>
+  <si>
+    <t>TCase_18</t>
+  </si>
+  <si>
+    <t>About_TProc_17</t>
+  </si>
+  <si>
+    <t>About_TProc_18</t>
+  </si>
+  <si>
+    <t>Check if the Register page can be directly navigated to from the About page as a non-logged in user</t>
+  </si>
+  <si>
+    <t>Check if the Log in page can be directly navigated to from the About page as a non-logged in user</t>
+  </si>
+  <si>
+    <t>Nav_TCon_15</t>
+  </si>
+  <si>
+    <t>Nav_TCon_16</t>
+  </si>
+  <si>
+    <t>Nav_TCon_17</t>
+  </si>
+  <si>
+    <t>Nav_TCon_18</t>
+  </si>
+  <si>
+    <t>User is directed to the Register page</t>
+  </si>
+  <si>
+    <t>User is directed to the Log in page</t>
+  </si>
+  <si>
+    <t>While on the About page and not logged in, select the Register link</t>
+  </si>
+  <si>
+    <t>While on the About page and not logged in, select the select the Log in link</t>
+  </si>
+  <si>
+    <t>TCase_19</t>
+  </si>
+  <si>
+    <t>About_TProc_19</t>
+  </si>
+  <si>
+    <t>Nav_TCon_19</t>
+  </si>
+  <si>
+    <t>Check if the My Account - reset password page can be directly navigated to from the About page as a logged in user</t>
+  </si>
+  <si>
+    <t>Check if a logged in user can log off from the About page</t>
+  </si>
+  <si>
+    <t>Check if the About page does not allow direct access to the "Forgot password" page</t>
+  </si>
+  <si>
+    <t>User is directed to the My Account - reset password  page</t>
+  </si>
+  <si>
+    <t>User is logged out of system.</t>
+  </si>
+  <si>
+    <t>User is unable to access Forgot password</t>
+  </si>
+  <si>
+    <t>While on the About page as a logged in user, select the My Account - reset password link</t>
+  </si>
+  <si>
+    <t>While on the About page as a logged in user, select the Log off link</t>
+  </si>
+  <si>
+    <t>While on the About page check if the Forgot password page is directly accessible</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1275,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1135,7 +1284,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1145,7 +1293,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1184,7 +1331,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
@@ -1210,7 +1357,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1307,11 +1453,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108670336"/>
-        <c:axId val="108676224"/>
+        <c:axId val="106835328"/>
+        <c:axId val="106841216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108670336"/>
+        <c:axId val="106835328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,7 +1466,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108676224"/>
+        <c:crossAx val="106841216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1328,7 +1474,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108676224"/>
+        <c:axId val="106841216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,7 +1485,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108670336"/>
+        <c:crossAx val="106835328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1745,10 +1891,10 @@
   <sheetPr>
     <tabColor rgb="FF023FAE"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,7 +1920,7 @@
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>59</v>
@@ -1791,7 +1937,7 @@
     </row>
     <row r="3" spans="1:9" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>60</v>
@@ -1806,10 +1952,10 @@
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>58</v>
@@ -1823,10 +1969,10 @@
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>58</v>
@@ -1840,10 +1986,10 @@
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>65</v>
@@ -1857,10 +2003,10 @@
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>183</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>66</v>
@@ -1874,10 +2020,10 @@
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>67</v>
+        <v>184</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>66</v>
@@ -1891,10 +2037,10 @@
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>69</v>
+        <v>185</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>66</v>
@@ -1905,13 +2051,13 @@
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -1919,13 +2065,13 @@
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -1933,27 +2079,27 @@
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -1961,16 +2107,71 @@
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -1998,8 +2199,8 @@
   </sheetPr>
   <dimension ref="A1:Z161"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D5"/>
+    <sheetView topLeftCell="A12" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2072,16 +2273,16 @@
     </row>
     <row r="2" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>61</v>
@@ -2096,7 +2297,7 @@
         <v>24</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
@@ -2111,16 +2312,16 @@
     </row>
     <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>62</v>
@@ -2135,7 +2336,7 @@
         <v>24</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
@@ -2150,16 +2351,16 @@
     </row>
     <row r="4" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>63</v>
@@ -2174,7 +2375,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="4"/>
@@ -2189,16 +2390,16 @@
     </row>
     <row r="5" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>64</v>
@@ -2213,7 +2414,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="4"/>
@@ -2225,19 +2426,19 @@
     </row>
     <row r="6" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>11</v>
@@ -2249,7 +2450,7 @@
         <v>24</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="4"/>
@@ -2261,19 +2462,19 @@
     </row>
     <row r="7" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>11</v>
@@ -2285,7 +2486,7 @@
         <v>24</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="4"/>
@@ -2300,19 +2501,19 @@
     </row>
     <row r="8" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>11</v>
@@ -2324,7 +2525,7 @@
         <v>24</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="4"/>
@@ -2338,24 +2539,24 @@
       </c>
       <c r="U8" s="30">
         <f>COUNTIF(H2:H90,"*Passed*")</f>
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>11</v>
@@ -2367,10 +2568,10 @@
         <v>25</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>33</v>
@@ -2383,7 +2584,7 @@
       </c>
       <c r="N9" s="10"/>
       <c r="O9" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P9" s="10"/>
       <c r="T9" t="s">
@@ -2396,19 +2597,19 @@
     </row>
     <row r="10" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>11</v>
@@ -2420,7 +2621,7 @@
         <v>24</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="4"/>
@@ -2439,19 +2640,19 @@
     </row>
     <row r="11" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>11</v>
@@ -2463,7 +2664,7 @@
         <v>24</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="4"/>
@@ -2475,19 +2676,19 @@
     </row>
     <row r="12" spans="1:26" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>11</v>
@@ -2499,10 +2700,10 @@
         <v>25</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>33</v>
@@ -2515,25 +2716,25 @@
       </c>
       <c r="N12" s="10"/>
       <c r="O12" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="P12" s="10"/>
     </row>
     <row r="13" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>27</v>
@@ -2545,7 +2746,7 @@
         <v>24</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -2557,19 +2758,19 @@
     </row>
     <row r="14" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>11</v>
@@ -2581,7 +2782,7 @@
         <v>24</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -2591,12 +2792,32 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="E15" s="10"/>
+    <row r="15" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>201</v>
+      </c>
       <c r="F15" s="11"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="10"/>
+      <c r="G15" s="31">
+        <v>42108</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
@@ -2605,12 +2826,32 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="E16" s="10"/>
+    <row r="16" spans="1:26" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="F16" s="11"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="10"/>
+      <c r="G16" s="31">
+        <v>42108</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
@@ -2619,12 +2860,32 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E17" s="10"/>
+    <row r="17" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="F17" s="11"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="10"/>
+      <c r="G17" s="31">
+        <v>42108</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
@@ -2633,12 +2894,32 @@
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E18" s="10"/>
+    <row r="18" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>218</v>
+      </c>
       <c r="F18" s="11"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="10"/>
+      <c r="G18" s="31">
+        <v>42108</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
@@ -2647,12 +2928,32 @@
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
     </row>
-    <row r="19" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E19" s="10"/>
+    <row r="19" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="F19" s="11"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="10"/>
+      <c r="G19" s="31">
+        <v>42108</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
@@ -2661,12 +2962,32 @@
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
     </row>
-    <row r="20" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E20" s="10"/>
+    <row r="20" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="F20" s="11"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="10"/>
+      <c r="G20" s="31">
+        <v>42108</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
@@ -2675,8 +2996,8 @@
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
     </row>
-    <row r="21" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E21" s="10"/>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
       <c r="F21" s="11"/>
       <c r="G21" s="10"/>
       <c r="H21" s="25"/>
@@ -2689,7 +3010,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
     </row>
-    <row r="22" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E22" s="10"/>
       <c r="F22" s="11"/>
       <c r="G22" s="10"/>
@@ -2703,7 +3024,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>
     </row>
-    <row r="23" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E23" s="10"/>
       <c r="F23" s="11"/>
       <c r="G23" s="10"/>
@@ -2717,7 +3038,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
     </row>
-    <row r="24" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E24" s="10"/>
       <c r="F24" s="11"/>
       <c r="G24" s="10"/>
@@ -2731,7 +3052,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E25" s="10"/>
       <c r="F25" s="11"/>
       <c r="G25" s="10"/>
@@ -2748,7 +3069,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E26" s="10"/>
       <c r="F26" s="11"/>
       <c r="G26" s="10"/>
@@ -2769,7 +3090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E27" s="10"/>
       <c r="F27" s="11"/>
       <c r="G27" s="10"/>
@@ -2790,7 +3111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E28" s="10"/>
       <c r="F28" s="11"/>
       <c r="G28" s="10"/>
@@ -2811,7 +3132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E29" s="10"/>
       <c r="F29" s="11"/>
       <c r="G29" s="10"/>
@@ -2832,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E30" s="10"/>
       <c r="F30" s="11"/>
       <c r="G30" s="10"/>
@@ -2853,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E31" s="10"/>
       <c r="F31" s="11"/>
       <c r="G31" s="10"/>
@@ -2867,7 +3188,7 @@
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E32" s="10"/>
       <c r="F32" s="11"/>
       <c r="G32" s="10"/>
@@ -4699,7 +5020,7 @@
   <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$A$4:$A$6</xm:f>
@@ -4710,7 +5031,7 @@
           <x14:formula1>
             <xm:f>Settings!$B$4:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F159</xm:sqref>
+          <xm:sqref>F2:F15 F18:F159</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -4724,6 +5045,12 @@
           </x14:formula1>
           <xm:sqref>K2:K12</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Settings!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>F16:F17</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -4735,10 +5062,10 @@
   <sheetPr>
     <tabColor rgb="FF99FF99"/>
   </sheetPr>
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4780,19 +5107,19 @@
     </row>
     <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="26" t="s">
@@ -4806,19 +5133,19 @@
     </row>
     <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
@@ -4831,19 +5158,19 @@
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -4856,19 +5183,19 @@
     </row>
     <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -4881,19 +5208,19 @@
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -4906,19 +5233,19 @@
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -4931,19 +5258,19 @@
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -4956,19 +5283,19 @@
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -4981,19 +5308,19 @@
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -5006,19 +5333,19 @@
     </row>
     <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -5031,19 +5358,19 @@
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -5056,19 +5383,19 @@
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -5081,19 +5408,19 @@
     </row>
     <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -5104,12 +5431,22 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -5119,12 +5456,22 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -5134,12 +5481,22 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -5149,12 +5506,22 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -5164,12 +5531,22 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -5178,6 +5555,23 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>177</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5272,21 +5666,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -5400,10 +5779,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -5418,16 +5819,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
priorities added to About
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 AboutPage, Kevin O'Hare.xlsx
+++ b/Testing Spreadsheet v1.0 AboutPage, Kevin O'Hare.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,8 @@
   <definedNames>
     <definedName name="_Toc407532261" localSheetId="0">Reqs!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -195,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="236">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -1453,11 +1454,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="106835328"/>
-        <c:axId val="106841216"/>
+        <c:axId val="105797120"/>
+        <c:axId val="105798656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="106835328"/>
+        <c:axId val="105797120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1466,7 +1467,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106841216"/>
+        <c:crossAx val="105798656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1474,7 +1475,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106841216"/>
+        <c:axId val="105798656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,7 +1486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106835328"/>
+        <c:crossAx val="105797120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1893,8 +1894,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2129,6 +2130,9 @@
       <c r="C15" s="1" t="s">
         <v>186</v>
       </c>
+      <c r="D15" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -2140,8 +2144,11 @@
       <c r="C16" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>193</v>
       </c>
@@ -2151,8 +2158,11 @@
       <c r="C17" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>194</v>
       </c>
@@ -2162,8 +2172,11 @@
       <c r="C18" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>195</v>
       </c>
@@ -2172,6 +2185,9 @@
       </c>
       <c r="C19" s="1" t="s">
         <v>192</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -5018,42 +5034,6 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Settings!$A$4:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H43</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Settings!$B$4:$B$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F15 F18:F159</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Settings!$F$4:$F$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>L2:L14</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Settings!$D$4:$D$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>K2:K12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]Settings!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>F16:F17</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5064,7 +5044,7 @@
   </sheetPr>
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -5666,6 +5646,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -5779,32 +5774,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -5819,9 +5792,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>